<commit_message>
I finally got a decent Model algorithm
</commit_message>
<xml_diff>
--- a/CH-118 DSO.xlsx
+++ b/CH-118 DSO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C78E88-C148-4588-BFF2-DD612CD51425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{BF44534F-910E-4EDC-B7CB-C8FFAAF33F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0F19A84-2C4F-4B65-B250-B8F6843D6F44}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="21">
   <si>
     <t>Result</t>
   </si>
@@ -115,6 +115,18 @@
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7244450548014350336/</t>
   </si>
+  <si>
+    <t>Days Out</t>
+  </si>
+  <si>
+    <t>Model Development</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>I like this approach</t>
+  </si>
 </sst>
 </file>
 
@@ -125,9 +137,9 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dddd"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0;\-0;0;@"/>
+    <numFmt numFmtId="166" formatCode="0;\-0;0;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +225,13 @@
       <name val="Garamond"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -416,13 +435,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -512,6 +532,11 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -521,14 +546,14 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Intro_Hd" xfId="3" xr:uid="{E7BBA5C7-3535-43FA-B02B-9829CA9D4357}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{60FBE962-0AD5-4744-8805-F21A700A4160}"/>
@@ -988,6 +1013,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1005,33 +1033,33 @@
       <selection activeCell="N21" sqref="N21:N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" customWidth="1"/>
     <col min="2" max="4" width="14" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="7" width="22.625" customWidth="1"/>
-    <col min="8" max="9" width="12.375" customWidth="1"/>
-    <col min="10" max="10" width="12.25" customWidth="1"/>
-    <col min="11" max="11" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.125" customWidth="1"/>
-    <col min="13" max="13" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.375" style="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.375" customWidth="1"/>
-    <col min="17" max="17" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" customWidth="1"/>
+    <col min="6" max="7" width="22.59765625" customWidth="1"/>
+    <col min="8" max="9" width="12.3984375" customWidth="1"/>
+    <col min="10" max="10" width="12.19921875" customWidth="1"/>
+    <col min="11" max="11" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.09765625" customWidth="1"/>
+    <col min="13" max="13" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.3984375" customWidth="1"/>
+    <col min="17" max="17" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="2:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="F1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="F1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="44"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1069,7 @@
       <c r="K1"/>
       <c r="N1" s="25"/>
     </row>
-    <row r="2" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1064,7 +1092,7 @@
       <c r="I2" s="3"/>
       <c r="P2" s="23"/>
     </row>
-    <row r="3" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12">
         <v>45368</v>
       </c>
@@ -1086,7 +1114,7 @@
       </c>
       <c r="I3" s="39"/>
     </row>
-    <row r="4" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B4" s="13">
         <v>45371</v>
       </c>
@@ -1108,7 +1136,7 @@
       </c>
       <c r="I4" s="40"/>
     </row>
-    <row r="5" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B5" s="13">
         <v>45380</v>
       </c>
@@ -1132,7 +1160,7 @@
       <c r="Q5" s="38"/>
       <c r="R5" s="26"/>
     </row>
-    <row r="6" spans="2:18" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="13">
         <v>45383</v>
       </c>
@@ -1151,7 +1179,7 @@
       <c r="Q6" s="29"/>
       <c r="R6" s="26"/>
     </row>
-    <row r="7" spans="2:18" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="18">
         <v>45385</v>
       </c>
@@ -1170,7 +1198,7 @@
       <c r="Q7" s="29"/>
       <c r="R7" s="26"/>
     </row>
-    <row r="8" spans="2:18" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="13">
         <v>45386</v>
       </c>
@@ -1188,7 +1216,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="26"/>
     </row>
-    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="13">
         <v>45407</v>
       </c>
@@ -1206,7 +1234,7 @@
       <c r="Q9" s="25"/>
       <c r="R9" s="26"/>
     </row>
-    <row r="10" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13">
         <v>45417</v>
       </c>
@@ -1221,7 +1249,7 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="26"/>
     </row>
-    <row r="11" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13">
         <v>45425</v>
       </c>
@@ -1239,7 +1267,7 @@
       <c r="Q11" s="25"/>
       <c r="R11" s="26"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" s="13">
         <v>45433</v>
       </c>
@@ -1254,7 +1282,7 @@
       <c r="Q12" s="25"/>
       <c r="R12" s="27"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B13" s="13">
         <v>45453</v>
       </c>
@@ -1269,7 +1297,7 @@
       <c r="I13" s="1"/>
       <c r="Q13" s="25"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B14" s="13">
         <v>45455</v>
       </c>
@@ -1285,7 +1313,7 @@
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B15" s="13">
         <v>45458</v>
       </c>
@@ -1305,7 +1333,7 @@
       <c r="P15" s="25"/>
       <c r="Q15" s="25"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B16" s="18">
         <v>45459</v>
       </c>
@@ -1325,7 +1353,7 @@
       <c r="P16" s="25"/>
       <c r="Q16" s="25"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B17" s="13">
         <v>45480</v>
       </c>
@@ -1338,17 +1366,17 @@
       <c r="E17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="45" t="s">
+      <c r="K17" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="48"/>
       <c r="P17" s="25"/>
       <c r="Q17" s="25"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B18" s="13">
         <v>45485</v>
       </c>
@@ -1368,7 +1396,7 @@
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B19" s="13">
         <v>45507</v>
       </c>
@@ -1393,7 +1421,7 @@
       <c r="P19" s="25"/>
       <c r="Q19" s="25"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B20" s="13">
         <v>45510</v>
       </c>
@@ -1423,7 +1451,7 @@
       </c>
       <c r="Q20" s="35"/>
     </row>
-    <row r="21" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="13">
         <v>45511</v>
       </c>
@@ -1454,7 +1482,7 @@
       </c>
       <c r="Q21" s="25"/>
     </row>
-    <row r="22" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="18">
         <v>45512</v>
       </c>
@@ -1484,7 +1512,7 @@
       </c>
       <c r="Q22" s="25"/>
     </row>
-    <row r="23" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="13">
         <v>45512</v>
       </c>
@@ -1514,7 +1542,7 @@
       </c>
       <c r="Q23" s="25"/>
     </row>
-    <row r="24" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>45516</v>
       </c>
@@ -1544,7 +1572,7 @@
       </c>
       <c r="Q24" s="25"/>
     </row>
-    <row r="25" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B25" s="13">
         <v>45529</v>
       </c>
@@ -1574,7 +1602,7 @@
       </c>
       <c r="Q25" s="35"/>
     </row>
-    <row r="26" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="K26" s="28">
         <v>45458</v>
       </c>
@@ -1592,7 +1620,7 @@
       </c>
       <c r="Q26" s="25"/>
     </row>
-    <row r="27" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="K27" s="28">
         <v>45453</v>
       </c>
@@ -1610,7 +1638,7 @@
       </c>
       <c r="Q27" s="25"/>
     </row>
-    <row r="28" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="K28" s="28">
         <v>45425</v>
       </c>
@@ -1628,7 +1656,7 @@
       </c>
       <c r="Q28" s="25"/>
     </row>
-    <row r="29" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B29" s="7"/>
       <c r="K29" s="30"/>
       <c r="L29" s="31"/>
@@ -1636,7 +1664,7 @@
       <c r="O29" s="31"/>
       <c r="Q29" s="25"/>
     </row>
-    <row r="30" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="K30" s="30"/>
       <c r="L30" s="31"/>
       <c r="M30" s="31"/>
@@ -1649,7 +1677,7 @@
       </c>
       <c r="Q30" s="25"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.35">
       <c r="K31" s="25"/>
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
@@ -1673,39 +1701,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C3B3CF-1900-4C46-93AC-2BD28E08A5EF}">
-  <dimension ref="B1:V38"/>
+  <dimension ref="B1:V49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F23" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" customWidth="1"/>
     <col min="2" max="4" width="14" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="7" width="22.625" customWidth="1"/>
-    <col min="8" max="13" width="12.375" customWidth="1"/>
-    <col min="14" max="14" width="12.25" customWidth="1"/>
-    <col min="15" max="15" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.125" customWidth="1"/>
-    <col min="17" max="17" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.375" style="25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.375" customWidth="1"/>
-    <col min="21" max="21" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" customWidth="1"/>
+    <col min="6" max="7" width="22.59765625" customWidth="1"/>
+    <col min="8" max="13" width="12.3984375" customWidth="1"/>
+    <col min="14" max="14" width="12.19921875" customWidth="1"/>
+    <col min="15" max="15" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.09765625" customWidth="1"/>
+    <col min="17" max="17" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.3984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.3984375" customWidth="1"/>
+    <col min="21" max="21" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="2:22" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="F1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="F1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="44"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1715,7 +1743,7 @@
       <c r="O1"/>
       <c r="R1" s="25"/>
     </row>
-    <row r="2" spans="2:22" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1742,7 +1770,7 @@
       <c r="M2" s="3"/>
       <c r="T2" s="23"/>
     </row>
-    <row r="3" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12">
         <v>45368</v>
       </c>
@@ -1768,7 +1796,7 @@
       <c r="L3" s="39"/>
       <c r="M3" s="39"/>
     </row>
-    <row r="4" spans="2:22" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B4" s="13">
         <v>45371</v>
       </c>
@@ -1794,7 +1822,7 @@
       <c r="L4" s="40"/>
       <c r="M4" s="40"/>
     </row>
-    <row r="5" spans="2:22" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B5" s="13">
         <v>45380</v>
       </c>
@@ -1822,7 +1850,7 @@
       <c r="U5" s="38"/>
       <c r="V5" s="26"/>
     </row>
-    <row r="6" spans="2:22" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="13">
         <v>45383</v>
       </c>
@@ -1845,7 +1873,7 @@
       <c r="U6" s="29"/>
       <c r="V6" s="26"/>
     </row>
-    <row r="7" spans="2:22" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="18">
         <v>45385</v>
       </c>
@@ -1868,7 +1896,7 @@
       <c r="U7" s="29"/>
       <c r="V7" s="26"/>
     </row>
-    <row r="8" spans="2:22" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="13">
         <v>45386</v>
       </c>
@@ -1879,7 +1907,9 @@
         <v>23360</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="50" t="s">
+        <v>18</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1890,7 +1920,7 @@
       <c r="U8" s="29"/>
       <c r="V8" s="26"/>
     </row>
-    <row r="9" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="13">
         <v>45407</v>
       </c>
@@ -1903,7 +1933,10 @@
       <c r="E9" s="5"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="5"/>
+      <c r="H9" s="51">
+        <f>M42</f>
+        <v>37.553661971830984</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -1912,7 +1945,7 @@
       <c r="U9" s="25"/>
       <c r="V9" s="26"/>
     </row>
-    <row r="10" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13">
         <v>45417</v>
       </c>
@@ -1923,11 +1956,18 @@
         <v>59716</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="str" cm="1">
+        <f t="array" ref="G10:G12">_xlfn._xlws.SORT(_xlfn.UNIQUE(C3:C25))</f>
+        <v>A</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="dataTable" ref="H10:H12" dt2D="0" dtr="0" r1="F42"/>
+        <v>37.553661971830984</v>
+      </c>
       <c r="U10" s="25"/>
       <c r="V10" s="26"/>
     </row>
-    <row r="11" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13">
         <v>45425</v>
       </c>
@@ -1939,8 +1979,12 @@
       </c>
       <c r="E11"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11"/>
+      <c r="G11" s="1" t="str">
+        <v>B</v>
+      </c>
+      <c r="H11">
+        <v>92.808335555555558</v>
+      </c>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1949,7 +1993,7 @@
       <c r="U11" s="25"/>
       <c r="V11" s="26"/>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B12" s="13">
         <v>45433</v>
       </c>
@@ -1960,11 +2004,16 @@
         <v>51253</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="str">
+        <v>C</v>
+      </c>
+      <c r="H12">
+        <v>61.12</v>
+      </c>
       <c r="U12" s="25"/>
       <c r="V12" s="27"/>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B13" s="13">
         <v>45453</v>
       </c>
@@ -1990,7 +2039,7 @@
       <c r="S13" s="42"/>
       <c r="U13" s="25"/>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B14" s="13">
         <v>45455</v>
       </c>
@@ -2014,7 +2063,7 @@
       <c r="T14" s="25"/>
       <c r="U14" s="25"/>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B15" s="13">
         <v>45458</v>
       </c>
@@ -2025,10 +2074,22 @@
         <v>95454</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="G15" s="8" t="str" cm="1">
+        <f t="array" aca="1" ref="G15:I18" ca="1">_xlfn.LET(_xlpm.z,_xlfn.XLOOKUP(_xlfn.ANCHORARRAY(G10),F3:F5,G3:G5),_xlfn.VSTACK({"Customer","Balance","DSO (day)"},_xlfn.HSTACK(_xlfn.ANCHORARRAY(G10),_xlpm.z,OFFSET(_xlfn.ANCHORARRAY(G10),,1))))</f>
+        <v>Customer</v>
+      </c>
+      <c r="H15" s="9" t="str">
+        <f ca="1"/>
+        <v>Balance</v>
+      </c>
+      <c r="I15" s="17" t="str">
+        <f ca="1"/>
+        <v>DSO (day)</v>
+      </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="O15" s="2"/>
@@ -2043,7 +2104,7 @@
       <c r="T15" s="25"/>
       <c r="U15" s="25"/>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B16" s="18">
         <v>45459</v>
       </c>
@@ -2054,12 +2115,31 @@
         <v>18000</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="G16" s="12" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="H16" s="10">
+        <f ca="1"/>
+        <v>355000</v>
+      </c>
+      <c r="I16" s="32">
+        <f ca="1"/>
+        <v>37.553661971830984</v>
+      </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="K16" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="K16:M18" ca="1">G16:I18=F3:H5</f>
+        <v>1</v>
+      </c>
+      <c r="L16" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M16" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
       <c r="O16" s="34" t="s">
         <v>1</v>
       </c>
@@ -2078,7 +2158,7 @@
       <c r="T16" s="25"/>
       <c r="U16" s="25"/>
     </row>
-    <row r="17" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B17" s="13">
         <v>45480</v>
       </c>
@@ -2089,12 +2169,31 @@
         <v>15131</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="G17" s="13" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="H17" s="11">
+        <f ca="1"/>
+        <v>450000</v>
+      </c>
+      <c r="I17" s="37">
+        <f ca="1"/>
+        <v>92.808335555555558</v>
+      </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+      <c r="K17" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="L17" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M17" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
       <c r="O17" s="28">
         <v>45529</v>
       </c>
@@ -2114,7 +2213,7 @@
       <c r="T17" s="25"/>
       <c r="U17" s="25"/>
     </row>
-    <row r="18" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B18" s="13">
         <v>45485</v>
       </c>
@@ -2125,12 +2224,31 @@
         <v>61430</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="G18" s="21" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+      <c r="H18" s="22">
+        <f ca="1"/>
+        <v>75000</v>
+      </c>
+      <c r="I18" s="36">
+        <f ca="1"/>
+        <v>61.12</v>
+      </c>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+      <c r="K18" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="L18" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M18" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
       <c r="O18" s="28">
         <v>45511</v>
       </c>
@@ -2149,7 +2267,7 @@
       <c r="T18" s="25"/>
       <c r="U18" s="25"/>
     </row>
-    <row r="19" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B19" s="13">
         <v>45507</v>
       </c>
@@ -2184,7 +2302,7 @@
       <c r="T19" s="25"/>
       <c r="U19" s="25"/>
     </row>
-    <row r="20" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B20" s="13">
         <v>45510</v>
       </c>
@@ -2218,7 +2336,7 @@
       </c>
       <c r="U20" s="35"/>
     </row>
-    <row r="21" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="13">
         <v>45511</v>
       </c>
@@ -2252,7 +2370,7 @@
       </c>
       <c r="U21" s="25"/>
     </row>
-    <row r="22" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="18">
         <v>45512</v>
       </c>
@@ -2286,7 +2404,7 @@
       </c>
       <c r="U22" s="25"/>
     </row>
-    <row r="23" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="13">
         <v>45512</v>
       </c>
@@ -2320,7 +2438,7 @@
       </c>
       <c r="U23" s="25"/>
     </row>
-    <row r="24" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>45516</v>
       </c>
@@ -2354,7 +2472,7 @@
       </c>
       <c r="U24" s="25"/>
     </row>
-    <row r="25" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B25" s="13">
         <v>45529</v>
       </c>
@@ -2377,7 +2495,7 @@
       <c r="S25" s="31"/>
       <c r="U25" s="35"/>
     </row>
-    <row r="26" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="O26" s="30"/>
       <c r="P26" s="31"/>
       <c r="Q26" s="31"/>
@@ -2390,199 +2508,501 @@
       </c>
       <c r="U26" s="25"/>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
       <c r="J27">
-        <f>_xlfn.XLOOKUP(F28,F3:F5,G3:G5)</f>
-        <v>75000</v>
-      </c>
-      <c r="K27" s="46">
+        <f>_xlfn.XLOOKUP(F28,$F$3:$F$5,$G$3:$G$5)</f>
+        <v>355000</v>
+      </c>
+      <c r="K27" s="43">
         <v>45535</v>
       </c>
-      <c r="L27" s="46"/>
-      <c r="M27" s="46"/>
+      <c r="L27" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="M27" s="43"/>
       <c r="U27" s="25"/>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
       <c r="F28" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G28" cm="1">
-        <f t="array" ref="G28:I31">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(B3:D25,C3:C25=F28),1,-1)</f>
-        <v>45512</v>
+        <f t="array" ref="G28:I35">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(B3:D25,C3:C25=F28),1,-1)</f>
+        <v>45529</v>
       </c>
       <c r="H28" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="I28">
-        <v>42000</v>
+        <v>79288</v>
       </c>
       <c r="J28">
         <f>IF(SUM($I$28:I28)&lt;$J$27,I28,$J$27-SUM($J27:J$28))</f>
-        <v>42000</v>
-      </c>
-      <c r="K28" s="47" cm="1">
-        <f t="array" ref="K28:K31">K27-_xlfn.TAKE(_xlfn.ANCHORARRAY(G28),,1)</f>
-        <v>23</v>
-      </c>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47" cm="1">
-        <f t="array" ref="M28:M31">_xlfn.LET(
-_xlpm.x, _xlfn.TAKE(_xlfn.ANCHORARRAY(G28),,-1),
-_xlfn.SCAN(0,_xlpm.x,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v))
+        <v>79288</v>
+      </c>
+      <c r="K28" s="44" cm="1">
+        <f t="array" ref="K28:K35">K27-_xlfn.TAKE(_xlfn.ANCHORARRAY(G28),,1)</f>
+        <v>6</v>
+      </c>
+      <c r="L28" s="44" cm="1">
+        <f t="array" ref="L28:L35">_xlfn.SCAN(0,
+_xlfn.TAKE(_xlfn.ANCHORARRAY(G28),,-1),
+_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v)
 )</f>
-        <v>42000</v>
+        <v>79288</v>
+      </c>
+      <c r="M28" s="44" cm="1">
+        <f t="array" ref="M28:M35">_xlfn.LET(_xlpm.z,$J$27-_xlfn.ANCHORARRAY(L28),IF(_xlpm.z&lt;0,0,_xlpm.z))</f>
+        <v>275712</v>
       </c>
       <c r="N28" cm="1">
-        <f t="array" ref="N28:N31">IF(_xlfn.ANCHORARRAY(M28)&lt;$J$27,I28:I31,$J$27-_xlfn.ANCHORARRAY(M28))</f>
-        <v>42000</v>
+        <f t="array" ref="N28:N35">_xlfn.LET(_xlpm.idx,_xlfn.XMATCH(0,_xlfn.ANCHORARRAY(M28)),_xlpm.d,_xlfn.ANCHORARRAY(M28),_xlpm.f,_xlfn.TAKE(_xlfn.ANCHORARRAY(G28),,-1),IF(_xlpm.d&gt;0,_xlpm.f,INDEX(_xlfn.ANCHORARRAY(M28),_xlpm.idx-1)))</f>
+        <v>79288</v>
+      </c>
+      <c r="O28" cm="1">
+        <f t="array" ref="O28:O35">IF(_xlfn.ANCHORARRAY(L28)&lt;$J$27,_xlfn.ANCHORARRAY(N28),$J$27-SUM(_xlfn.ANCHORARRAY(L28)))</f>
+        <v>79288</v>
       </c>
       <c r="U28" s="25"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
       <c r="G29">
-        <v>45459</v>
+        <v>45511</v>
       </c>
       <c r="H29" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="I29">
-        <v>18000</v>
+        <v>75300</v>
       </c>
       <c r="J29">
         <f>IF(SUM($I$28:I29)&lt;$J$27,I29,$J$27-SUM($J28:J$28))</f>
-        <v>18000</v>
-      </c>
-      <c r="K29" s="47">
-        <v>76</v>
-      </c>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47">
-        <v>60000</v>
+        <v>75300</v>
+      </c>
+      <c r="K29" s="44">
+        <v>24</v>
+      </c>
+      <c r="L29" s="44">
+        <v>154588</v>
+      </c>
+      <c r="M29" s="44">
+        <v>200412</v>
       </c>
       <c r="N29">
-        <v>18000</v>
+        <v>75300</v>
+      </c>
+      <c r="O29">
+        <v>75300</v>
       </c>
       <c r="U29" s="25"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
       <c r="G30">
-        <v>45385</v>
+        <v>45510</v>
       </c>
       <c r="H30" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="I30">
-        <v>15000</v>
+        <v>65995</v>
       </c>
       <c r="J30">
         <f>IF(SUM($I$28:I30)&lt;$J$27,I30,$J$27-SUM($J$28:J29))</f>
-        <v>15000</v>
-      </c>
-      <c r="K30" s="47">
-        <v>150</v>
-      </c>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47">
-        <v>75000</v>
+        <v>65995</v>
+      </c>
+      <c r="K30" s="44">
+        <v>25</v>
+      </c>
+      <c r="L30" s="44">
+        <v>220583</v>
+      </c>
+      <c r="M30" s="44">
+        <v>134417</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>65995</v>
+      </c>
+      <c r="O30">
+        <v>65995</v>
       </c>
       <c r="U30" s="25"/>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
       <c r="G31">
-        <v>45371</v>
+        <v>45507</v>
       </c>
       <c r="H31" t="str">
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="I31">
-        <v>25883</v>
+        <v>13660</v>
       </c>
       <c r="J31">
         <f>IF(SUM($I$28:I31)&lt;$J$27,I31,$J$27-SUM($J$28:J30))</f>
-        <v>0</v>
-      </c>
-      <c r="K31" s="47">
-        <v>164</v>
-      </c>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47">
-        <v>100883</v>
+        <v>13660</v>
+      </c>
+      <c r="K31" s="44">
+        <v>28</v>
+      </c>
+      <c r="L31" s="44">
+        <v>234243</v>
+      </c>
+      <c r="M31" s="44">
+        <v>120757</v>
       </c>
       <c r="N31">
-        <v>-25883</v>
-      </c>
-      <c r="O31" s="25"/>
+        <v>13660</v>
+      </c>
+      <c r="O31" s="25">
+        <v>13660</v>
+      </c>
       <c r="P31" s="25"/>
       <c r="Q31" s="25"/>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <v>45480</v>
+      </c>
+      <c r="H32" t="str">
+        <v>A</v>
+      </c>
+      <c r="I32">
+        <v>15131</v>
+      </c>
       <c r="J32">
         <f>IF(SUM($I$28:I32)&lt;$J$27,I32,$J$27-SUM($J$28:J31))</f>
-        <v>0</v>
-      </c>
-      <c r="K32" s="47"/>
+        <v>15131</v>
+      </c>
+      <c r="K32" s="44">
+        <v>55</v>
+      </c>
       <c r="L32">
+        <v>249374</v>
+      </c>
+      <c r="M32">
+        <v>105626</v>
+      </c>
+      <c r="N32">
+        <v>15131</v>
+      </c>
+      <c r="O32">
+        <v>15131</v>
+      </c>
+      <c r="P32">
         <f>SUMPRODUCT(J28:J38,K28:K38)/$J$27</f>
-        <v>61.12</v>
-      </c>
-    </row>
-    <row r="33" spans="10:13" x14ac:dyDescent="0.3">
+        <v>37.553661971830984</v>
+      </c>
+    </row>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>45458</v>
+      </c>
+      <c r="H33" t="str">
+        <v>A</v>
+      </c>
+      <c r="I33">
+        <v>95454</v>
+      </c>
       <c r="J33">
         <f>IF(SUM($I$28:I33)&lt;$J$27,I33,$J$27-SUM($J$28:J32))</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-    </row>
-    <row r="34" spans="10:13" x14ac:dyDescent="0.3">
+        <v>95454</v>
+      </c>
+      <c r="K33" s="44">
+        <v>77</v>
+      </c>
+      <c r="L33" s="44">
+        <v>344828</v>
+      </c>
+      <c r="M33" s="44">
+        <v>10172</v>
+      </c>
+      <c r="N33">
+        <v>95454</v>
+      </c>
+      <c r="O33">
+        <v>95454</v>
+      </c>
+    </row>
+    <row r="34" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <v>45453</v>
+      </c>
+      <c r="H34" t="str">
+        <v>A</v>
+      </c>
+      <c r="I34">
+        <v>80241</v>
+      </c>
       <c r="J34">
         <f>IF(SUM($I$28:I34)&lt;$J$27,I34,$J$27-SUM($J$28:J33))</f>
+        <v>10172</v>
+      </c>
+      <c r="K34" s="44">
+        <v>82</v>
+      </c>
+      <c r="L34" s="44">
+        <v>425069</v>
+      </c>
+      <c r="M34" s="44">
         <v>0</v>
       </c>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-    </row>
-    <row r="35" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="N34">
+        <v>10172</v>
+      </c>
+      <c r="O34">
+        <v>-1790662</v>
+      </c>
+    </row>
+    <row r="35" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <v>45425</v>
+      </c>
+      <c r="H35" t="str">
+        <v>A</v>
+      </c>
+      <c r="I35">
+        <v>12620</v>
+      </c>
       <c r="J35">
         <f>IF(SUM($I$28:I35)&lt;$J$27,I35,$J$27-SUM($J$28:J34))</f>
         <v>0</v>
       </c>
-      <c r="K35" s="47"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-    </row>
-    <row r="36" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="K35" s="44">
+        <v>110</v>
+      </c>
+      <c r="L35" s="44">
+        <v>437689</v>
+      </c>
+      <c r="M35" s="44">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>10172</v>
+      </c>
+      <c r="O35">
+        <v>-1790662</v>
+      </c>
+    </row>
+    <row r="36" spans="5:15" x14ac:dyDescent="0.35">
       <c r="J36">
         <f>IF(SUM($I$28:I36)&lt;$J$27,I36,$J$27-SUM($J$28:J35))</f>
         <v>0</v>
       </c>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-    </row>
-    <row r="37" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="44"/>
+    </row>
+    <row r="37" spans="5:15" x14ac:dyDescent="0.35">
       <c r="J37">
         <f>IF(SUM($I$28:I37)&lt;$J$27,I37,$J$27-SUM($J$28:J36))</f>
         <v>0</v>
       </c>
-      <c r="K37" s="47"/>
-      <c r="L37" s="47"/>
-      <c r="M37" s="47"/>
-    </row>
-    <row r="38" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+    </row>
+    <row r="38" spans="5:15" x14ac:dyDescent="0.35">
       <c r="J38">
         <f>IF(SUM($I$28:I38)&lt;$J$27,I38,$J$27-SUM($J$28:J37))</f>
         <v>0</v>
       </c>
-      <c r="K38" s="47"/>
-      <c r="L38" s="47"/>
-      <c r="M38" s="47"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="44"/>
+    </row>
+    <row r="39" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+    </row>
+    <row r="40" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E40" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40">
+        <f>_xlfn.XLOOKUP(F42,$F$3:$F$5,$G$3:$G$5)</f>
+        <v>355000</v>
+      </c>
+      <c r="L40" s="43">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="41" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="J41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" cm="1">
+        <f t="array" ref="G42:I49">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(B3:D25,C3:C25=F42),1,-1)</f>
+        <v>45529</v>
+      </c>
+      <c r="H42" t="str">
+        <v>A</v>
+      </c>
+      <c r="I42">
+        <v>79288</v>
+      </c>
+      <c r="J42" s="49" cm="1">
+        <f t="array" ref="J42:J49">K27-_xlfn.TAKE(_xlfn.ANCHORARRAY(G42),,1)</f>
+        <v>6</v>
+      </c>
+      <c r="K42" cm="1">
+        <f t="array" ref="K42:K49">_xlfn.DROP(_xlfn.VSTACK(K40,_xlfn.LET(_xlpm.d,$K$40-_xlfn.SCAN(0,_xlfn.TAKE(_xlfn.ANCHORARRAY(G42),,-1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v)),IF(_xlpm.d&lt;0,0,_xlpm.d))),-1)</f>
+        <v>355000</v>
+      </c>
+      <c r="L42" cm="1">
+        <f t="array" ref="L42:L49">_xlfn.MAP(_xlfn.TAKE(_xlfn.ANCHORARRAY(G42),,-1),_xlfn.ANCHORARRAY(K42),_xlfn.LAMBDA(_xlpm.x,_xlpm.y,MIN(_xlpm.x,_xlpm.y)))</f>
+        <v>79288</v>
+      </c>
+      <c r="M42">
+        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(J42),_xlfn.ANCHORARRAY(L42))/$K$40</f>
+        <v>37.553661971830984</v>
+      </c>
+    </row>
+    <row r="43" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>45511</v>
+      </c>
+      <c r="H43" t="str">
+        <v>A</v>
+      </c>
+      <c r="I43">
+        <v>75300</v>
+      </c>
+      <c r="J43" s="49">
+        <v>24</v>
+      </c>
+      <c r="K43">
+        <v>275712</v>
+      </c>
+      <c r="L43">
+        <v>75300</v>
+      </c>
+    </row>
+    <row r="44" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>45510</v>
+      </c>
+      <c r="H44" t="str">
+        <v>A</v>
+      </c>
+      <c r="I44">
+        <v>65995</v>
+      </c>
+      <c r="J44" s="49">
+        <v>25</v>
+      </c>
+      <c r="K44">
+        <v>200412</v>
+      </c>
+      <c r="L44">
+        <v>65995</v>
+      </c>
+    </row>
+    <row r="45" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>45507</v>
+      </c>
+      <c r="H45" t="str">
+        <v>A</v>
+      </c>
+      <c r="I45">
+        <v>13660</v>
+      </c>
+      <c r="J45" s="49">
+        <v>28</v>
+      </c>
+      <c r="K45">
+        <v>134417</v>
+      </c>
+      <c r="L45">
+        <v>13660</v>
+      </c>
+    </row>
+    <row r="46" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <v>45480</v>
+      </c>
+      <c r="H46" t="str">
+        <v>A</v>
+      </c>
+      <c r="I46">
+        <v>15131</v>
+      </c>
+      <c r="J46" s="49">
+        <v>55</v>
+      </c>
+      <c r="K46">
+        <v>120757</v>
+      </c>
+      <c r="L46">
+        <v>15131</v>
+      </c>
+    </row>
+    <row r="47" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <v>45458</v>
+      </c>
+      <c r="H47" t="str">
+        <v>A</v>
+      </c>
+      <c r="I47">
+        <v>95454</v>
+      </c>
+      <c r="J47" s="49">
+        <v>77</v>
+      </c>
+      <c r="K47">
+        <v>105626</v>
+      </c>
+      <c r="L47">
+        <v>95454</v>
+      </c>
+    </row>
+    <row r="48" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>45453</v>
+      </c>
+      <c r="H48" t="str">
+        <v>A</v>
+      </c>
+      <c r="I48">
+        <v>80241</v>
+      </c>
+      <c r="J48" s="49">
+        <v>82</v>
+      </c>
+      <c r="K48">
+        <v>10172</v>
+      </c>
+      <c r="L48">
+        <v>10172</v>
+      </c>
+    </row>
+    <row r="49" spans="7:12" x14ac:dyDescent="0.35">
+      <c r="G49">
+        <v>45425</v>
+      </c>
+      <c r="H49" t="str">
+        <v>A</v>
+      </c>
+      <c r="I49">
+        <v>12620</v>
+      </c>
+      <c r="J49" s="49">
+        <v>110</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2598,37 +3018,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842FD16E-83AA-4CA9-8818-67DB9D7BCA8A}">
   <dimension ref="B1:R39"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" customWidth="1"/>
     <col min="2" max="4" width="14" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="7" width="22.625" customWidth="1"/>
-    <col min="8" max="9" width="12.375" customWidth="1"/>
-    <col min="10" max="10" width="12.25" customWidth="1"/>
-    <col min="11" max="11" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.125" customWidth="1"/>
-    <col min="13" max="13" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.375" style="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.375" customWidth="1"/>
-    <col min="17" max="17" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" customWidth="1"/>
+    <col min="6" max="7" width="22.59765625" customWidth="1"/>
+    <col min="8" max="9" width="12.3984375" customWidth="1"/>
+    <col min="10" max="10" width="12.19921875" customWidth="1"/>
+    <col min="11" max="11" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.09765625" customWidth="1"/>
+    <col min="13" max="13" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.3984375" customWidth="1"/>
+    <col min="17" max="17" width="12.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="2:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="F1" s="44" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="F1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="44"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +3058,7 @@
       <c r="K1"/>
       <c r="N1" s="25"/>
     </row>
-    <row r="2" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2661,7 +3081,7 @@
       <c r="I2" s="3"/>
       <c r="P2" s="23"/>
     </row>
-    <row r="3" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12">
         <v>45368</v>
       </c>
@@ -2683,7 +3103,7 @@
       </c>
       <c r="I3" s="39"/>
     </row>
-    <row r="4" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B4" s="13">
         <v>45371</v>
       </c>
@@ -2705,7 +3125,7 @@
       </c>
       <c r="I4" s="40"/>
     </row>
-    <row r="5" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B5" s="13">
         <v>45380</v>
       </c>
@@ -2729,7 +3149,7 @@
       <c r="Q5" s="38"/>
       <c r="R5" s="26"/>
     </row>
-    <row r="6" spans="2:18" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="13">
         <v>45383</v>
       </c>
@@ -2748,7 +3168,7 @@
       <c r="Q6" s="29"/>
       <c r="R6" s="26"/>
     </row>
-    <row r="7" spans="2:18" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="18">
         <v>45385</v>
       </c>
@@ -2767,7 +3187,7 @@
       <c r="Q7" s="29"/>
       <c r="R7" s="26"/>
     </row>
-    <row r="8" spans="2:18" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="13">
         <v>45386</v>
       </c>
@@ -2785,7 +3205,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="26"/>
     </row>
-    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="13">
         <v>45407</v>
       </c>
@@ -2803,7 +3223,7 @@
       <c r="Q9" s="25"/>
       <c r="R9" s="26"/>
     </row>
-    <row r="10" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13">
         <v>45417</v>
       </c>
@@ -2818,7 +3238,7 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="26"/>
     </row>
-    <row r="11" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13">
         <v>45425</v>
       </c>
@@ -2836,7 +3256,7 @@
       <c r="Q11" s="25"/>
       <c r="R11" s="26"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" s="13">
         <v>45433</v>
       </c>
@@ -2851,7 +3271,7 @@
       <c r="Q12" s="25"/>
       <c r="R12" s="27"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B13" s="13">
         <v>45453</v>
       </c>
@@ -2866,7 +3286,7 @@
       <c r="I13" s="1"/>
       <c r="Q13" s="25"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B14" s="13">
         <v>45455</v>
       </c>
@@ -2882,7 +3302,7 @@
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B15" s="13">
         <v>45458</v>
       </c>
@@ -2902,7 +3322,7 @@
       <c r="P15" s="25"/>
       <c r="Q15" s="25"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B16" s="18">
         <v>45459</v>
       </c>
@@ -2922,7 +3342,7 @@
       <c r="P16" s="25"/>
       <c r="Q16" s="25"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B17" s="13">
         <v>45480</v>
       </c>
@@ -2935,17 +3355,17 @@
       <c r="E17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="45" t="s">
+      <c r="K17" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="48"/>
       <c r="P17" s="25"/>
       <c r="Q17" s="25"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B18" s="13">
         <v>45485</v>
       </c>
@@ -2965,7 +3385,7 @@
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B19" s="13">
         <v>45507</v>
       </c>
@@ -2990,7 +3410,7 @@
       <c r="P19" s="25"/>
       <c r="Q19" s="25"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B20" s="13">
         <v>45510</v>
       </c>
@@ -3020,7 +3440,7 @@
       </c>
       <c r="Q20" s="35"/>
     </row>
-    <row r="21" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="13">
         <v>45511</v>
       </c>
@@ -3051,7 +3471,7 @@
       </c>
       <c r="Q21" s="25"/>
     </row>
-    <row r="22" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B22" s="18">
         <v>45512</v>
       </c>
@@ -3081,7 +3501,7 @@
       </c>
       <c r="Q22" s="25"/>
     </row>
-    <row r="23" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B23" s="13">
         <v>45512</v>
       </c>
@@ -3111,7 +3531,7 @@
       </c>
       <c r="Q23" s="25"/>
     </row>
-    <row r="24" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
         <v>45516</v>
       </c>
@@ -3141,7 +3561,7 @@
       </c>
       <c r="Q24" s="25"/>
     </row>
-    <row r="25" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B25" s="13">
         <v>45529</v>
       </c>
@@ -3171,7 +3591,7 @@
       </c>
       <c r="Q25" s="35"/>
     </row>
-    <row r="26" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="K26" s="28">
         <v>45458</v>
       </c>
@@ -3189,7 +3609,7 @@
       </c>
       <c r="Q26" s="25"/>
     </row>
-    <row r="27" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="K27" s="28">
         <v>45453</v>
       </c>
@@ -3207,7 +3627,7 @@
       </c>
       <c r="Q27" s="25"/>
     </row>
-    <row r="28" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="K28" s="28">
         <v>45425</v>
       </c>
@@ -3225,7 +3645,7 @@
       </c>
       <c r="Q28" s="25"/>
     </row>
-    <row r="29" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B29" s="7"/>
       <c r="K29" s="30"/>
       <c r="L29" s="31"/>
@@ -3233,7 +3653,7 @@
       <c r="O29" s="31"/>
       <c r="Q29" s="25"/>
     </row>
-    <row r="30" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="K30" s="30"/>
       <c r="L30" s="31"/>
       <c r="M30" s="31"/>
@@ -3246,14 +3666,14 @@
       </c>
       <c r="Q30" s="25"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.35">
       <c r="K31" s="25"/>
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
       <c r="O31" s="25"/>
     </row>
-    <row r="32" spans="2:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="48" cm="1">
+    <row r="32" spans="2:17" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="45" cm="1">
         <f t="array" ref="B32:B34">_xlfn.MAP(
     F3:F5,
     G3:G5,
@@ -3292,7 +3712,7 @@
         <v>275712</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
         <v>92.808335555555558</v>
       </c>
@@ -3300,7 +3720,7 @@
         <v>200412</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
         <v>61.12</v>
       </c>
@@ -3308,27 +3728,27 @@
         <v>134417</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D35" s="4">
         <v>120757</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D36" s="4">
         <v>105626</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D37" s="4">
         <v>10172</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D38" s="4">
         <v>-70069</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D39" s="4">
         <v>-82689</v>
       </c>

</xml_diff>

<commit_message>
Done. I now understand how to solve this problem.
</commit_message>
<xml_diff>
--- a/CH-118 DSO.xlsx
+++ b/CH-118 DSO.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{BF44534F-910E-4EDC-B7CB-C8FFAAF33F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0F19A84-2C4F-4B65-B250-B8F6843D6F44}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="8_{BF44534F-910E-4EDC-B7CB-C8FFAAF33F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E89F3118-DA78-440E-9241-0A132E5997A1}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="4" r:id="rId3"/>
+    <sheet name="SingleFunction" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="24">
   <si>
     <t>Result</t>
   </si>
@@ -126,6 +127,15 @@
   </si>
   <si>
     <t>I like this approach</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
+    <t>My Single Function</t>
   </si>
 </sst>
 </file>
@@ -442,7 +452,7 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -537,6 +547,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -546,10 +560,9 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -1051,15 +1064,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="F1" s="47" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="F1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="47"/>
+      <c r="G1" s="51"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1366,13 +1379,13 @@
       <c r="E17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="48" t="s">
+      <c r="K17" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
       <c r="P17" s="25"/>
       <c r="Q17" s="25"/>
     </row>
@@ -1703,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C3B3CF-1900-4C46-93AC-2BD28E08A5EF}">
   <dimension ref="B1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1725,15 +1738,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="F1" s="47" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="F1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="47"/>
+      <c r="G1" s="51"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1907,7 +1920,7 @@
         <v>23360</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="47" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="1"/>
@@ -1933,7 +1946,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="51">
+      <c r="H9" s="48">
         <f>M42</f>
         <v>37.553661971830984</v>
       </c>
@@ -2817,7 +2830,7 @@
       <c r="M39" s="44"/>
     </row>
     <row r="40" spans="5:15" x14ac:dyDescent="0.35">
-      <c r="E40" s="52" t="s">
+      <c r="E40" s="49" t="s">
         <v>20</v>
       </c>
       <c r="K40">
@@ -2847,7 +2860,7 @@
       <c r="I42">
         <v>79288</v>
       </c>
-      <c r="J42" s="49" cm="1">
+      <c r="J42" s="46" cm="1">
         <f t="array" ref="J42:J49">K27-_xlfn.TAKE(_xlfn.ANCHORARRAY(G42),,1)</f>
         <v>6</v>
       </c>
@@ -2874,7 +2887,7 @@
       <c r="I43">
         <v>75300</v>
       </c>
-      <c r="J43" s="49">
+      <c r="J43" s="46">
         <v>24</v>
       </c>
       <c r="K43">
@@ -2894,7 +2907,7 @@
       <c r="I44">
         <v>65995</v>
       </c>
-      <c r="J44" s="49">
+      <c r="J44" s="46">
         <v>25</v>
       </c>
       <c r="K44">
@@ -2914,7 +2927,7 @@
       <c r="I45">
         <v>13660</v>
       </c>
-      <c r="J45" s="49">
+      <c r="J45" s="46">
         <v>28</v>
       </c>
       <c r="K45">
@@ -2934,7 +2947,7 @@
       <c r="I46">
         <v>15131</v>
       </c>
-      <c r="J46" s="49">
+      <c r="J46" s="46">
         <v>55</v>
       </c>
       <c r="K46">
@@ -2954,7 +2967,7 @@
       <c r="I47">
         <v>95454</v>
       </c>
-      <c r="J47" s="49">
+      <c r="J47" s="46">
         <v>77</v>
       </c>
       <c r="K47">
@@ -2974,7 +2987,7 @@
       <c r="I48">
         <v>80241</v>
       </c>
-      <c r="J48" s="49">
+      <c r="J48" s="46">
         <v>82</v>
       </c>
       <c r="K48">
@@ -2994,7 +3007,7 @@
       <c r="I49">
         <v>12620</v>
       </c>
-      <c r="J49" s="49">
+      <c r="J49" s="46">
         <v>110</v>
       </c>
       <c r="K49">
@@ -3016,7 +3029,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{842FD16E-83AA-4CA9-8818-67DB9D7BCA8A}">
-  <dimension ref="B1:R39"/>
+  <dimension ref="B1:R34"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
@@ -3040,15 +3053,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="F1" s="47" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="F1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="47"/>
+      <c r="G1" s="51"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3355,13 +3368,13 @@
       <c r="E17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="48" t="s">
+      <c r="K17" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
       <c r="P17" s="25"/>
       <c r="Q17" s="25"/>
     </row>
@@ -3673,7 +3686,7 @@
       <c r="O31" s="25"/>
     </row>
     <row r="32" spans="2:17" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="45" cm="1">
+      <c r="B32" s="45" t="e" cm="1">
         <f t="array" ref="B32:B34">_xlfn.MAP(
     F3:F5,
     G3:G5,
@@ -3692,10 +3705,10 @@
         )
     )
 )</f>
-        <v>37.553661971830984</v>
-      </c>
-      <c r="D32" s="4" cm="1">
-        <f t="array" ref="D32:D39">_xlfn.LET(
+        <v>#NAME?</v>
+      </c>
+      <c r="D32" s="4" t="e" cm="1">
+        <f t="array" ref="D32">_xlfn.LET(
     _xlpm.A,"A",
     _xlpm.B,355000,
             _xlpm.T, _xlfn._xlws.SORT(B3:D25, , -1),
@@ -3709,48 +3722,17 @@
             _xlpm.V, _xlfn.VSTACK(_xlfn.TAKE(_xlpm.I, _xlpm.X - 1), INDEX(_xlpm.R, _xlpm.X - 1)),
            _xlpm.R
 )</f>
-        <v>275712</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="4">
-        <v>92.808335555555558</v>
-      </c>
-      <c r="D33" s="4">
-        <v>200412</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="4">
-        <v>61.12</v>
-      </c>
-      <c r="D34" s="4">
-        <v>134417</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D35" s="4">
-        <v>120757</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D36" s="4">
-        <v>105626</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D37" s="4">
-        <v>10172</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D38" s="4">
-        <v>-70069</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="D39" s="4">
-        <v>-82689</v>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="4" t="e">
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="4" t="e">
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -3762,4 +3744,1405 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5948BA-F5E8-4739-9E31-66FDA022F863}">
+  <dimension ref="B1:V54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.19921875" customWidth="1"/>
+    <col min="2" max="4" width="14" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" customWidth="1"/>
+    <col min="6" max="7" width="22.59765625" customWidth="1"/>
+    <col min="8" max="13" width="12.3984375" customWidth="1"/>
+    <col min="14" max="14" width="12.19921875" customWidth="1"/>
+    <col min="15" max="15" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.09765625" customWidth="1"/>
+    <col min="17" max="17" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.3984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.3984375" customWidth="1"/>
+    <col min="21" max="21" width="12.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="F1" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="51"/>
+      <c r="H1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1"/>
+      <c r="R1" s="25"/>
+    </row>
+    <row r="2" spans="2:22" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="T2" s="23"/>
+    </row>
+    <row r="3" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="12">
+        <v>45368</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="10">
+        <v>91647</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="10">
+        <v>355000</v>
+      </c>
+      <c r="H3" s="32">
+        <v>37.553661971830984</v>
+      </c>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+    </row>
+    <row r="4" spans="2:22" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B4" s="13">
+        <v>45371</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="11">
+        <v>25883</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="11">
+        <v>450000</v>
+      </c>
+      <c r="H4" s="37">
+        <v>92.808335555555558</v>
+      </c>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+    </row>
+    <row r="5" spans="2:22" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+      <c r="B5" s="13">
+        <v>45380</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="11">
+        <v>25273</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="22">
+        <v>75000</v>
+      </c>
+      <c r="H5" s="36">
+        <v>61.12</v>
+      </c>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="26"/>
+    </row>
+    <row r="6" spans="2:22" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="13">
+        <v>45383</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="11">
+        <v>32927</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="26"/>
+    </row>
+    <row r="7" spans="2:22" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="18">
+        <v>45385</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="20">
+        <v>15000</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="26"/>
+    </row>
+    <row r="8" spans="2:22" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="13">
+        <v>45386</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="11">
+        <v>23360</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="26"/>
+    </row>
+    <row r="9" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="13">
+        <v>45407</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="11">
+        <v>65558</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="48">
+        <f>M42</f>
+        <v>37.553661971830984</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="26"/>
+    </row>
+    <row r="10" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="13">
+        <v>45417</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="11">
+        <v>59716</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="str" cm="1">
+        <f t="array" ref="G10:G12">_xlfn._xlws.SORT(_xlfn.UNIQUE(C3:C25))</f>
+        <v>A</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="dataTable" ref="H10:H12" dt2D="0" dtr="0" r1="F42"/>
+        <v>37.553661971830984</v>
+      </c>
+      <c r="U10" s="25"/>
+      <c r="V10" s="26"/>
+    </row>
+    <row r="11" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="13">
+        <v>45425</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="11">
+        <v>12620</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="str">
+        <v>B</v>
+      </c>
+      <c r="H11">
+        <v>92.808335555555558</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="26"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B12" s="13">
+        <v>45433</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="11">
+        <v>51253</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="str">
+        <v>C</v>
+      </c>
+      <c r="H12">
+        <v>61.12</v>
+      </c>
+      <c r="U12" s="25"/>
+      <c r="V12" s="27"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B13" s="13">
+        <v>45453</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="11">
+        <v>80241</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="O13" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="U13" s="25"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B14" s="13">
+        <v>45455</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="11">
+        <v>16485</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B15" s="13">
+        <v>45458</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="11">
+        <v>95454</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="G15" s="8" t="str" cm="1">
+        <f t="array" aca="1" ref="G15:I18" ca="1">_xlfn.LET(_xlpm.z,_xlfn.XLOOKUP(_xlfn.ANCHORARRAY(G10),F3:F5,G3:G5),_xlfn.VSTACK({"Customer","Balance","DSO (day)"},_xlfn.HSTACK(_xlfn.ANCHORARRAY(G10),_xlpm.z,OFFSET(_xlfn.ANCHORARRAY(G10),,1))))</f>
+        <v>Customer</v>
+      </c>
+      <c r="H15" s="9" t="str">
+        <f ca="1"/>
+        <v>Balance</v>
+      </c>
+      <c r="I15" s="17" t="str">
+        <f ca="1"/>
+        <v>DSO (day)</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" s="33">
+        <v>45535</v>
+      </c>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B16" s="18">
+        <v>45459</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="20">
+        <v>18000</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="G16" s="12" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="H16" s="10">
+        <f ca="1"/>
+        <v>355000</v>
+      </c>
+      <c r="I16" s="32">
+        <f ca="1"/>
+        <v>37.553661971830984</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1" t="b" cm="1">
+        <f t="array" aca="1" ref="K16:M18" ca="1">G16:I18=F3:H5</f>
+        <v>1</v>
+      </c>
+      <c r="L16" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M16" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="S16" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+    </row>
+    <row r="17" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="13">
+        <v>45480</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="11">
+        <v>15131</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="G17" s="13" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="H17" s="11">
+        <f ca="1"/>
+        <v>450000</v>
+      </c>
+      <c r="I17" s="37">
+        <f ca="1"/>
+        <v>92.808335555555558</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="L17" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M17" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="O17" s="28">
+        <v>45529</v>
+      </c>
+      <c r="P17" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="29">
+        <v>79288</v>
+      </c>
+      <c r="R17" s="25">
+        <v>79288</v>
+      </c>
+      <c r="S17" s="29" cm="1">
+        <f t="array" ref="S17:S24">S15-O17:O24</f>
+        <v>6</v>
+      </c>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+    </row>
+    <row r="18" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="13">
+        <v>45485</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="11">
+        <v>61430</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="G18" s="21" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+      <c r="H18" s="22">
+        <f ca="1"/>
+        <v>75000</v>
+      </c>
+      <c r="I18" s="36">
+        <f ca="1"/>
+        <v>61.12</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="L18" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="M18" s="1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="28">
+        <v>45511</v>
+      </c>
+      <c r="P18" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="29">
+        <v>75300</v>
+      </c>
+      <c r="R18" s="25">
+        <v>75300</v>
+      </c>
+      <c r="S18" s="29">
+        <v>24</v>
+      </c>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25"/>
+    </row>
+    <row r="19" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="13">
+        <v>45507</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="11">
+        <v>13660</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="O19" s="28">
+        <v>45510</v>
+      </c>
+      <c r="P19" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="29">
+        <v>65995</v>
+      </c>
+      <c r="R19" s="25">
+        <v>65995</v>
+      </c>
+      <c r="S19" s="29">
+        <v>25</v>
+      </c>
+      <c r="T19" s="25"/>
+      <c r="U19" s="25"/>
+    </row>
+    <row r="20" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="13">
+        <v>45510</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="11">
+        <v>65995</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="O20" s="28">
+        <v>45507</v>
+      </c>
+      <c r="P20" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="29">
+        <v>13660</v>
+      </c>
+      <c r="R20" s="25">
+        <v>13660</v>
+      </c>
+      <c r="S20" s="29">
+        <v>28</v>
+      </c>
+      <c r="U20" s="35"/>
+    </row>
+    <row r="21" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="13">
+        <v>45511</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="11">
+        <v>75300</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="O21" s="28">
+        <v>45480</v>
+      </c>
+      <c r="P21" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="29">
+        <v>15131</v>
+      </c>
+      <c r="R21" s="25">
+        <v>15131</v>
+      </c>
+      <c r="S21" s="29">
+        <v>55</v>
+      </c>
+      <c r="U21" s="25"/>
+    </row>
+    <row r="22" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="18">
+        <v>45512</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="20">
+        <v>42000</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="O22" s="28">
+        <v>45458</v>
+      </c>
+      <c r="P22" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="29">
+        <v>95454</v>
+      </c>
+      <c r="R22" s="25">
+        <v>95454</v>
+      </c>
+      <c r="S22" s="29">
+        <v>77</v>
+      </c>
+      <c r="U22" s="25"/>
+    </row>
+    <row r="23" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="13">
+        <v>45512</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="11">
+        <v>21649</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="O23" s="28">
+        <v>45453</v>
+      </c>
+      <c r="P23" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="29">
+        <v>80241</v>
+      </c>
+      <c r="R23" s="25">
+        <v>10172</v>
+      </c>
+      <c r="S23" s="29">
+        <v>82</v>
+      </c>
+      <c r="U23" s="25"/>
+    </row>
+    <row r="24" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="13">
+        <v>45516</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="11">
+        <v>78482</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="O24" s="28">
+        <v>45425</v>
+      </c>
+      <c r="P24" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="29">
+        <v>12620</v>
+      </c>
+      <c r="R24" s="25">
+        <v>0</v>
+      </c>
+      <c r="S24" s="29">
+        <v>110</v>
+      </c>
+      <c r="U24" s="25"/>
+    </row>
+    <row r="25" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="13">
+        <v>45529</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="11">
+        <v>79288</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="U25" s="35"/>
+    </row>
+    <row r="26" spans="2:21" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="O26" s="30"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="S26" s="41">
+        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(S17),R17:R24)/SUM(R17:R24)</f>
+        <v>37.553661971830984</v>
+      </c>
+      <c r="U26" s="25"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="J27">
+        <f>_xlfn.XLOOKUP(F28,$F$3:$F$5,$G$3:$G$5)</f>
+        <v>355000</v>
+      </c>
+      <c r="K27" s="43">
+        <v>45535</v>
+      </c>
+      <c r="L27" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="M27" s="43"/>
+      <c r="U27" s="25"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="F28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" cm="1">
+        <f t="array" ref="G28:I35">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(B3:D25,C3:C25=F28),1,-1)</f>
+        <v>45529</v>
+      </c>
+      <c r="H28" t="str">
+        <v>A</v>
+      </c>
+      <c r="I28">
+        <v>79288</v>
+      </c>
+      <c r="J28">
+        <f>IF(SUM($I$28:I28)&lt;$J$27,I28,$J$27-SUM($J27:J$28))</f>
+        <v>79288</v>
+      </c>
+      <c r="K28" s="44" cm="1">
+        <f t="array" ref="K28:K35">K27-_xlfn.TAKE(_xlfn.ANCHORARRAY(G28),,1)</f>
+        <v>6</v>
+      </c>
+      <c r="L28" s="44" cm="1">
+        <f t="array" ref="L28:L35">_xlfn.SCAN(0,
+_xlfn.TAKE(_xlfn.ANCHORARRAY(G28),,-1),
+_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v)
+)</f>
+        <v>79288</v>
+      </c>
+      <c r="M28" s="44" cm="1">
+        <f t="array" ref="M28:M35">_xlfn.LET(_xlpm.z,$J$27-_xlfn.ANCHORARRAY(L28),IF(_xlpm.z&lt;0,0,_xlpm.z))</f>
+        <v>275712</v>
+      </c>
+      <c r="N28" cm="1">
+        <f t="array" ref="N28:N35">_xlfn.LET(_xlpm.idx,_xlfn.XMATCH(0,_xlfn.ANCHORARRAY(M28)),_xlpm.d,_xlfn.ANCHORARRAY(M28),_xlpm.f,_xlfn.TAKE(_xlfn.ANCHORARRAY(G28),,-1),IF(_xlpm.d&gt;0,_xlpm.f,INDEX(_xlfn.ANCHORARRAY(M28),_xlpm.idx-1)))</f>
+        <v>79288</v>
+      </c>
+      <c r="O28" cm="1">
+        <f t="array" ref="O28:O35">IF(_xlfn.ANCHORARRAY(L28)&lt;$J$27,_xlfn.ANCHORARRAY(N28),$J$27-SUM(_xlfn.ANCHORARRAY(L28)))</f>
+        <v>79288</v>
+      </c>
+      <c r="U28" s="25"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <v>45511</v>
+      </c>
+      <c r="H29" t="str">
+        <v>A</v>
+      </c>
+      <c r="I29">
+        <v>75300</v>
+      </c>
+      <c r="J29">
+        <f>IF(SUM($I$28:I29)&lt;$J$27,I29,$J$27-SUM($J28:J$28))</f>
+        <v>75300</v>
+      </c>
+      <c r="K29" s="44">
+        <v>24</v>
+      </c>
+      <c r="L29" s="44">
+        <v>154588</v>
+      </c>
+      <c r="M29" s="44">
+        <v>200412</v>
+      </c>
+      <c r="N29">
+        <v>75300</v>
+      </c>
+      <c r="O29">
+        <v>75300</v>
+      </c>
+      <c r="U29" s="25"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <v>45510</v>
+      </c>
+      <c r="H30" t="str">
+        <v>A</v>
+      </c>
+      <c r="I30">
+        <v>65995</v>
+      </c>
+      <c r="J30">
+        <f>IF(SUM($I$28:I30)&lt;$J$27,I30,$J$27-SUM($J$28:J29))</f>
+        <v>65995</v>
+      </c>
+      <c r="K30" s="44">
+        <v>25</v>
+      </c>
+      <c r="L30" s="44">
+        <v>220583</v>
+      </c>
+      <c r="M30" s="44">
+        <v>134417</v>
+      </c>
+      <c r="N30">
+        <v>65995</v>
+      </c>
+      <c r="O30">
+        <v>65995</v>
+      </c>
+      <c r="U30" s="25"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <v>45507</v>
+      </c>
+      <c r="H31" t="str">
+        <v>A</v>
+      </c>
+      <c r="I31">
+        <v>13660</v>
+      </c>
+      <c r="J31">
+        <f>IF(SUM($I$28:I31)&lt;$J$27,I31,$J$27-SUM($J$28:J30))</f>
+        <v>13660</v>
+      </c>
+      <c r="K31" s="44">
+        <v>28</v>
+      </c>
+      <c r="L31" s="44">
+        <v>234243</v>
+      </c>
+      <c r="M31" s="44">
+        <v>120757</v>
+      </c>
+      <c r="N31">
+        <v>13660</v>
+      </c>
+      <c r="O31" s="25">
+        <v>13660</v>
+      </c>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+      <c r="S31" s="25"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <v>45480</v>
+      </c>
+      <c r="H32" t="str">
+        <v>A</v>
+      </c>
+      <c r="I32">
+        <v>15131</v>
+      </c>
+      <c r="J32">
+        <f>IF(SUM($I$28:I32)&lt;$J$27,I32,$J$27-SUM($J$28:J31))</f>
+        <v>15131</v>
+      </c>
+      <c r="K32" s="44">
+        <v>55</v>
+      </c>
+      <c r="L32">
+        <v>249374</v>
+      </c>
+      <c r="M32">
+        <v>105626</v>
+      </c>
+      <c r="N32">
+        <v>15131</v>
+      </c>
+      <c r="O32">
+        <v>15131</v>
+      </c>
+      <c r="P32">
+        <f>SUMPRODUCT(J28:J38,K28:K38)/$J$27</f>
+        <v>37.553661971830984</v>
+      </c>
+    </row>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>45458</v>
+      </c>
+      <c r="H33" t="str">
+        <v>A</v>
+      </c>
+      <c r="I33">
+        <v>95454</v>
+      </c>
+      <c r="J33">
+        <f>IF(SUM($I$28:I33)&lt;$J$27,I33,$J$27-SUM($J$28:J32))</f>
+        <v>95454</v>
+      </c>
+      <c r="K33" s="44">
+        <v>77</v>
+      </c>
+      <c r="L33" s="44">
+        <v>344828</v>
+      </c>
+      <c r="M33" s="44">
+        <v>10172</v>
+      </c>
+      <c r="N33">
+        <v>95454</v>
+      </c>
+      <c r="O33">
+        <v>95454</v>
+      </c>
+    </row>
+    <row r="34" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <v>45453</v>
+      </c>
+      <c r="H34" t="str">
+        <v>A</v>
+      </c>
+      <c r="I34">
+        <v>80241</v>
+      </c>
+      <c r="J34">
+        <f>IF(SUM($I$28:I34)&lt;$J$27,I34,$J$27-SUM($J$28:J33))</f>
+        <v>10172</v>
+      </c>
+      <c r="K34" s="44">
+        <v>82</v>
+      </c>
+      <c r="L34" s="44">
+        <v>425069</v>
+      </c>
+      <c r="M34" s="44">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>10172</v>
+      </c>
+      <c r="O34">
+        <v>-1790662</v>
+      </c>
+    </row>
+    <row r="35" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <v>45425</v>
+      </c>
+      <c r="H35" t="str">
+        <v>A</v>
+      </c>
+      <c r="I35">
+        <v>12620</v>
+      </c>
+      <c r="J35">
+        <f>IF(SUM($I$28:I35)&lt;$J$27,I35,$J$27-SUM($J$28:J34))</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="44">
+        <v>110</v>
+      </c>
+      <c r="L35" s="44">
+        <v>437689</v>
+      </c>
+      <c r="M35" s="44">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>10172</v>
+      </c>
+      <c r="O35">
+        <v>-1790662</v>
+      </c>
+    </row>
+    <row r="36" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="J36">
+        <f>IF(SUM($I$28:I36)&lt;$J$27,I36,$J$27-SUM($J$28:J35))</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="44"/>
+    </row>
+    <row r="37" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="J37">
+        <f>IF(SUM($I$28:I37)&lt;$J$27,I37,$J$27-SUM($J$28:J36))</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+    </row>
+    <row r="38" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="J38">
+        <f>IF(SUM($I$28:I38)&lt;$J$27,I38,$J$27-SUM($J$28:J37))</f>
+        <v>0</v>
+      </c>
+      <c r="K38" s="44"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="44"/>
+    </row>
+    <row r="39" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+    </row>
+    <row r="40" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E40" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40">
+        <f>_xlfn.XLOOKUP(F42,$F$3:$F$5,$G$3:$G$5)</f>
+        <v>355000</v>
+      </c>
+      <c r="L40" s="43">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="41" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="J41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" cm="1">
+        <f t="array" ref="G42:I49">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(B3:D25,C3:C25=F42),1,-1)</f>
+        <v>45529</v>
+      </c>
+      <c r="H42" t="str">
+        <v>A</v>
+      </c>
+      <c r="I42">
+        <v>79288</v>
+      </c>
+      <c r="J42" s="46" cm="1">
+        <f t="array" ref="J42:J49">K27-_xlfn.TAKE(_xlfn.ANCHORARRAY(G42),,1)</f>
+        <v>6</v>
+      </c>
+      <c r="K42" cm="1">
+        <f t="array" ref="K42:K49">_xlfn.DROP(_xlfn.VSTACK(K40,_xlfn.LET(_xlpm.d,$K$40-_xlfn.SCAN(0,_xlfn.TAKE(_xlfn.ANCHORARRAY(G42),,-1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v)),IF(_xlpm.d&lt;0,0,_xlpm.d))),-1)</f>
+        <v>355000</v>
+      </c>
+      <c r="L42" cm="1">
+        <f t="array" ref="L42:L49">_xlfn.MAP(_xlfn.TAKE(_xlfn.ANCHORARRAY(G42),,-1),_xlfn.ANCHORARRAY(K42),_xlfn.LAMBDA(_xlpm.x,_xlpm.y,MIN(_xlpm.x,_xlpm.y)))</f>
+        <v>79288</v>
+      </c>
+      <c r="M42">
+        <f>SUMPRODUCT(_xlfn.ANCHORARRAY(J42),_xlfn.ANCHORARRAY(L42))/$K$40</f>
+        <v>37.553661971830984</v>
+      </c>
+    </row>
+    <row r="43" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>45511</v>
+      </c>
+      <c r="H43" t="str">
+        <v>A</v>
+      </c>
+      <c r="I43">
+        <v>75300</v>
+      </c>
+      <c r="J43" s="46">
+        <v>24</v>
+      </c>
+      <c r="K43">
+        <v>275712</v>
+      </c>
+      <c r="L43">
+        <v>75300</v>
+      </c>
+    </row>
+    <row r="44" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>45510</v>
+      </c>
+      <c r="H44" t="str">
+        <v>A</v>
+      </c>
+      <c r="I44">
+        <v>65995</v>
+      </c>
+      <c r="J44" s="46">
+        <v>25</v>
+      </c>
+      <c r="K44">
+        <v>200412</v>
+      </c>
+      <c r="L44">
+        <v>65995</v>
+      </c>
+    </row>
+    <row r="45" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>45507</v>
+      </c>
+      <c r="H45" t="str">
+        <v>A</v>
+      </c>
+      <c r="I45">
+        <v>13660</v>
+      </c>
+      <c r="J45" s="46">
+        <v>28</v>
+      </c>
+      <c r="K45">
+        <v>134417</v>
+      </c>
+      <c r="L45">
+        <v>13660</v>
+      </c>
+    </row>
+    <row r="46" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <v>45480</v>
+      </c>
+      <c r="H46" t="str">
+        <v>A</v>
+      </c>
+      <c r="I46">
+        <v>15131</v>
+      </c>
+      <c r="J46" s="46">
+        <v>55</v>
+      </c>
+      <c r="K46">
+        <v>120757</v>
+      </c>
+      <c r="L46">
+        <v>15131</v>
+      </c>
+    </row>
+    <row r="47" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <v>45458</v>
+      </c>
+      <c r="H47" t="str">
+        <v>A</v>
+      </c>
+      <c r="I47">
+        <v>95454</v>
+      </c>
+      <c r="J47" s="46">
+        <v>77</v>
+      </c>
+      <c r="K47">
+        <v>105626</v>
+      </c>
+      <c r="L47">
+        <v>95454</v>
+      </c>
+    </row>
+    <row r="48" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>45453</v>
+      </c>
+      <c r="H48" t="str">
+        <v>A</v>
+      </c>
+      <c r="I48">
+        <v>80241</v>
+      </c>
+      <c r="J48" s="46">
+        <v>82</v>
+      </c>
+      <c r="K48">
+        <v>10172</v>
+      </c>
+      <c r="L48">
+        <v>10172</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="G49">
+        <v>45425</v>
+      </c>
+      <c r="H49" t="str">
+        <v>A</v>
+      </c>
+      <c r="I49">
+        <v>12620</v>
+      </c>
+      <c r="J49" s="46">
+        <v>110</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C50" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="J50" t="s">
+        <v>22</v>
+      </c>
+      <c r="K50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E51" s="8" t="str" cm="1">
+        <f t="array" aca="1" ref="E51:G54" ca="1">_xlfn.LET(
+_xlpm.x, _xlfn._xlws.SORT(B3:D25,1,-1),
+_xlpm.u, _xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.x,2)),
+_xlpm.fd,_xlfn.LAMBDA(_xlpm.ds,_xlpm.dc,_xlpm.ds-_xlpm.dc),
+_xlpm.fr,_xlfn.LAMBDA(_xlpm.p,_xlpm.sc, _xlfn.DROP(_xlfn.VSTACK(_xlpm.p,_xlfn.LET(_xlpm.d,_xlpm.p-_xlfn.SCAN(0,_xlfn.TAKE(_xlpm.sc,,-1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v)),IF(_xlpm.d&lt;0,0,_xlpm.d))),-1)),
+_xlpm.fx,_xlfn.LAMBDA(_xlpm.rc,_xlpm.sc,_xlfn.MAP(_xlpm.sc,_xlpm.rc,_xlfn.LAMBDA(_xlpm.x,_xlpm.y,MIN(_xlpm.x,_xlpm.y)))),
+_xlpm.z, _xlfn.REDUCE(0,_xlpm.u,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.LET(
+                          _xlpm.d, _xlfn._xlws.FILTER(_xlpm.x,_xlfn.CHOOSECOLS(_xlpm.x,2)=_xlpm.v),
+                          _xlpm.p, _xlfn.XLOOKUP(_xlpm.v,$G$16:$G$18,$H$16:$H$18),
+                          _xlpm.ds, _xlfn.TAKE(_xlpm.d,,-1),
+                          _xlpm.dc, _xlfn.TAKE(_xlpm.d,,1),
+                          _xlpm.do, _xlpm.fd($L$40,_xlpm.dc),
+                          _xlpm.r,  _xlpm.fx(_xlpm.fr(_xlpm.p,_xlpm.ds),_xlpm.ds),
+                          _xlpm.z, SUMPRODUCT(_xlpm.do,_xlpm.r)/_xlpm.p,
+                          _xlfn.VSTACK(_xlpm.a,_xlpm.z)
+                         )
+                 )
+      ),
+_xlfn.VSTACK(G15:I15,_xlfn.HSTACK(_xlpm.u,_xlfn.XLOOKUP(_xlpm.u,$G$16:$G$18,$H$16:$H$18),_xlfn.DROP(_xlpm.z,1)))
+)</f>
+        <v>Customer</v>
+      </c>
+      <c r="F51" s="9" t="str">
+        <f ca="1"/>
+        <v>Balance</v>
+      </c>
+      <c r="G51" s="17" t="str">
+        <f ca="1"/>
+        <v>DSO (day)</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E52" s="12" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="F52" s="10">
+        <f ca="1"/>
+        <v>355000</v>
+      </c>
+      <c r="G52" s="32">
+        <f ca="1"/>
+        <v>37.553661971830984</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E53" s="13" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="F53" s="11">
+        <f ca="1"/>
+        <v>450000</v>
+      </c>
+      <c r="G53" s="37">
+        <f ca="1"/>
+        <v>92.808335555555558</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="E54" s="21" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+      <c r="F54" s="22">
+        <f ca="1"/>
+        <v>75000</v>
+      </c>
+      <c r="G54" s="36">
+        <f ca="1"/>
+        <v>61.12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tried a new way of commenting functions
</commit_message>
<xml_diff>
--- a/CH-118 DSO.xlsx
+++ b/CH-118 DSO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="8_{BF44534F-910E-4EDC-B7CB-C8FFAAF33F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E89F3118-DA78-440E-9241-0A132E5997A1}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="8_{BF44534F-910E-4EDC-B7CB-C8FFAAF33F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0950B1F-80EE-4154-978F-7125477EAD76}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,6 +551,9 @@
     <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -558,9 +561,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1064,15 +1064,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="F1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="51"/>
+      <c r="G1" s="52"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1379,13 +1379,13 @@
       <c r="E17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="52" t="s">
+      <c r="K17" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
-      <c r="O17" s="52"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
       <c r="P17" s="25"/>
       <c r="Q17" s="25"/>
     </row>
@@ -1738,15 +1738,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="F1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="51"/>
+      <c r="G1" s="52"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3053,15 +3053,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="F1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="51"/>
+      <c r="G1" s="52"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -3368,13 +3368,13 @@
       <c r="E17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="K17" s="52" t="s">
+      <c r="K17" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
-      <c r="O17" s="52"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
       <c r="P17" s="25"/>
       <c r="Q17" s="25"/>
     </row>
@@ -3750,8 +3750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5948BA-F5E8-4739-9E31-66FDA022F863}">
   <dimension ref="B1:V54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3772,15 +3772,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="F1" s="51" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="F1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="51"/>
+      <c r="G1" s="52"/>
       <c r="H1" s="16" t="s">
         <v>0</v>
       </c>
@@ -5052,7 +5052,7 @@
       </c>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C50" s="53" t="s">
+      <c r="C50" s="50" t="s">
         <v>23</v>
       </c>
       <c r="J50" t="s">
@@ -5064,26 +5064,34 @@
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.35">
       <c r="E51" s="8" t="str" cm="1">
-        <f t="array" aca="1" ref="E51:G54" ca="1">_xlfn.LET(
-_xlpm.x, _xlfn._xlws.SORT(B3:D25,1,-1),
-_xlpm.u, _xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.x,2)),
-_xlpm.fd,_xlfn.LAMBDA(_xlpm.ds,_xlpm.dc,_xlpm.ds-_xlpm.dc),
-_xlpm.fr,_xlfn.LAMBDA(_xlpm.p,_xlpm.sc, _xlfn.DROP(_xlfn.VSTACK(_xlpm.p,_xlfn.LET(_xlpm.d,_xlpm.p-_xlfn.SCAN(0,_xlfn.TAKE(_xlpm.sc,,-1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v)),IF(_xlpm.d&lt;0,0,_xlpm.d))),-1)),
-_xlpm.fx,_xlfn.LAMBDA(_xlpm.rc,_xlpm.sc,_xlfn.MAP(_xlpm.sc,_xlpm.rc,_xlfn.LAMBDA(_xlpm.x,_xlpm.y,MIN(_xlpm.x,_xlpm.y)))),
-_xlpm.z, _xlfn.REDUCE(0,_xlpm.u,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.LET(
-                          _xlpm.d, _xlfn._xlws.FILTER(_xlpm.x,_xlfn.CHOOSECOLS(_xlpm.x,2)=_xlpm.v),
-                          _xlpm.p, _xlfn.XLOOKUP(_xlpm.v,$G$16:$G$18,$H$16:$H$18),
-                          _xlpm.ds, _xlfn.TAKE(_xlpm.d,,-1),
-                          _xlpm.dc, _xlfn.TAKE(_xlpm.d,,1),
-                          _xlpm.do, _xlpm.fd($L$40,_xlpm.dc),
-                          _xlpm.r,  _xlpm.fx(_xlpm.fr(_xlpm.p,_xlpm.ds),_xlpm.ds),
-                          _xlpm.z, SUMPRODUCT(_xlpm.do,_xlpm.r)/_xlpm.p,
-                          _xlfn.VSTACK(_xlpm.a,_xlpm.z)
-                         )
-                 )
-      ),
-_xlfn.VSTACK(G15:I15,_xlfn.HSTACK(_xlpm.u,_xlfn.XLOOKUP(_xlpm.u,$G$16:$G$18,$H$16:$H$18),_xlfn.DROP(_xlpm.z,1)))
-)</f>
+        <f t="array" aca="1" ref="E51:G54" ca="1">_xlfn.LAMBDA(_xlpm.data,_xlpm.cust,_xlpm.bal,_xlpm.date,
+   _xlfn.LET(
+       _xlpm.c_1, "Sorting the data so the latest sales is at the bottom of the list",
+            _xlpm.x, _xlfn._xlws.SORT(_xlpm.data,1,-1),
+       _xlpm.c_2, "Make a list of all the unique customers",
+            _xlpm.u, _xlfn.UNIQUE(_xlfn.CHOOSECOLS(_xlpm.x,2)),
+       _xlpm.c_3, "Function to generate number of days to the end point",
+            _xlpm.fd,_xlfn.LAMBDA(_xlpm.ds,_xlpm.dc,_xlpm.ds-_xlpm.dc),
+       _xlpm.c_4, "List of the remaining unmatched revenue immediately prior to apply a new sales value",
+            _xlpm.fr,_xlfn.LAMBDA(_xlpm.p,_xlpm.sc, _xlfn.DROP(_xlfn.VSTACK(_xlpm.p,_xlfn.LET(_xlpm.d,_xlpm.p-_xlfn.SCAN(0,_xlfn.TAKE(_xlpm.sc,,-1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlpm.a+_xlpm.v)),IF(_xlpm.d&lt;0,0,_xlpm.d))),-1)),
+       _xlpm.c_5, "List of payment matches amount to each sale",
+            _xlpm.fx,_xlfn.LAMBDA(_xlpm.rc,_xlpm.sc,_xlfn.MAP(_xlpm.sc,_xlpm.rc,_xlfn.LAMBDA(_xlpm.x,_xlpm.y,MIN(_xlpm.x,_xlpm.y)))),
+       _xlpm.c_6, "Okay, use reduce to process each customer",
+            _xlpm.z, _xlfn.REDUCE(0,_xlpm.u,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.LET(
+                                   _xlpm.d, _xlfn._xlws.FILTER(_xlpm.x,_xlfn.CHOOSECOLS(_xlpm.x,2)=_xlpm.v),
+                                   _xlpm.p, _xlfn.XLOOKUP(_xlpm.v,_xlpm.cust,_xlpm.bal),
+                                   _xlpm.ds, _xlfn.TAKE(_xlpm.d,,-1),
+                                   _xlpm.dc, _xlfn.TAKE(_xlpm.d,,1),
+                                   _xlpm.do, _xlpm.fd(_xlpm.date,_xlpm.dc),
+                                   _xlpm.r,  _xlpm.fx(_xlpm.fr(_xlpm.p,_xlpm.ds),_xlpm.ds),
+                                   _xlpm.z, SUMPRODUCT(_xlpm.do,_xlpm.r)/_xlpm.p,
+                                   _xlfn.VSTACK(_xlpm.a,_xlpm.z)
+                                 )
+                          )
+              ),
+               _xlfn.VSTACK(G15:I15,_xlfn.HSTACK(_xlpm.u,_xlfn.XLOOKUP(_xlpm.u,_xlpm.cust,_xlpm.bal),_xlfn.DROP(_xlpm.z,1)))
+      )
+)(B3:D25,G16:G18, H16:H18,L40)</f>
         <v>Customer</v>
       </c>
       <c r="F51" s="9" t="str">

</xml_diff>